<commit_message>
bugfix_neglect the last TC in TB
</commit_message>
<xml_diff>
--- a/case_support_testBatch.xlsx
+++ b/case_support_testBatch.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="244" yWindow="111" windowWidth="14810" windowHeight="7322" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7320" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="GLOBAL_CONFIG" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="520">
   <si>
     <t>SCAN_AP</t>
   </si>
@@ -1848,7 +1848,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1864,7 +1864,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1906,7 +1906,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1941,7 +1941,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2158,8 +2158,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.8984375" customWidth="1"/>
-    <col min="2" max="2" width="21.69921875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2634,8 +2634,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.3984375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2982,7 +2982,7 @@
         <v>5002</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
       <c r="B39" s="29" t="s">
         <v>349</v>
@@ -3105,8 +3105,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.8984375" customWidth="1"/>
-    <col min="3" max="3" width="55.3984375" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" customWidth="1"/>
+    <col min="3" max="3" width="55.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3535,19 +3535,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.09765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.8984375" customWidth="1"/>
-    <col min="14" max="14" width="21.8984375" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="14" max="14" width="21.88671875" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="14.69921875" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
@@ -5514,7 +5514,7 @@
       <c r="AM32" s="29"/>
       <c r="AN32" s="29"/>
     </row>
-    <row r="33" spans="1:40" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:40" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
         <v>119</v>
       </c>
@@ -6840,7 +6840,7 @@
       <c r="AM51" s="29"/>
       <c r="AN51" s="29"/>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:40" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>154</v>
       </c>
@@ -6910,7 +6910,7 @@
       <c r="AM52" s="29"/>
       <c r="AN52" s="29"/>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:40" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>162</v>
       </c>
@@ -6976,7 +6976,7 @@
       <c r="AM53" s="29"/>
       <c r="AN53" s="29"/>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:40" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
         <v>161</v>
       </c>
@@ -7668,7 +7668,7 @@
       <c r="AM65" s="29"/>
       <c r="AN65" s="29"/>
     </row>
-    <row r="66" spans="1:40" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:40" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A66" s="28" t="s">
         <v>149</v>
       </c>
@@ -8587,13 +8587,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.69921875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.69921875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.69921875" customWidth="1"/>
-    <col min="11" max="12" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" customWidth="1"/>
+    <col min="11" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
@@ -9630,7 +9630,7 @@
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
     </row>
-    <row r="45" spans="1:14" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
         <v>31</v>
       </c>
@@ -9710,7 +9710,7 @@
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
     </row>
-    <row r="49" spans="1:14" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
         <v>32</v>
       </c>
@@ -9860,7 +9860,7 @@
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>35</v>
       </c>
@@ -10727,7 +10727,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A92" s="24" t="s">
         <v>330</v>
       </c>
@@ -10905,7 +10905,7 @@
       <c r="M100" s="29"/>
       <c r="N100" s="29"/>
     </row>
-    <row r="101" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" s="27" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A101" s="24" t="s">
         <v>410</v>
       </c>
@@ -11038,21 +11038,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.296875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.296875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="6.69921875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="10.296875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.296875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="16.8984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.8984375" style="12"/>
-    <col min="11" max="11" width="10.296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.09765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="8.8984375" style="12"/>
-    <col min="17" max="18" width="12.69921875" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.69921875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.8984375" style="11"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.88671875" style="12"/>
+    <col min="11" max="11" width="10.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="8.88671875" style="12"/>
+    <col min="17" max="18" width="12.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
@@ -11717,7 +11717,7 @@
       <c r="T19" s="23"/>
       <c r="U19" s="23"/>
     </row>
-    <row r="20" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="86.4" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
@@ -12250,7 +12250,7 @@
       <c r="T38" s="23"/>
       <c r="U38" s="23"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>475</v>
       </c>
@@ -13137,7 +13137,7 @@
       <c r="T69" s="23"/>
       <c r="U69" s="23"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A70" s="28" t="s">
         <v>483</v>
       </c>
@@ -13392,19 +13392,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomLeft" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.296875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.8984375" style="13"/>
-    <col min="3" max="3" width="21.59765625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="8.8984375" style="13"/>
-    <col min="10" max="10" width="15.8984375" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.8984375" style="13"/>
-    <col min="14" max="14" width="11.296875" style="13" customWidth="1"/>
-    <col min="15" max="16384" width="8.8984375" style="13"/>
+    <col min="1" max="1" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="13"/>
+    <col min="3" max="3" width="21.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="8.88671875" style="13"/>
+    <col min="10" max="10" width="15.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.88671875" style="13"/>
+    <col min="14" max="14" width="11.33203125" style="13" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="32" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
@@ -13698,13 +13698,61 @@
       <c r="N11" s="28"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N12" s="28"/>
+      <c r="C12" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="K12" s="13">
+        <v>4</v>
+      </c>
+      <c r="L12" s="13">
+        <v>5</v>
+      </c>
+      <c r="M12" s="13">
+        <v>6</v>
+      </c>
+      <c r="N12" s="28" t="s">
+        <v>513</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="P12" s="13">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>1122</v>
+      </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N13" s="28"/>
+      <c r="N13" s="28" t="s">
+        <v>513</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="P13" s="13">
+        <v>555</v>
+      </c>
+      <c r="Q13" s="13">
+        <v>666</v>
+      </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N14" s="28"/>
+      <c r="N14" s="28" t="s">
+        <v>509</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>519</v>
+      </c>
+      <c r="P14" s="13">
+        <v>1111</v>
+      </c>
+      <c r="Q14" s="13">
+        <v>2222</v>
+      </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N15" s="28"/>

</xml_diff>